<commit_message>
Added filtering to "calls". Tests included. Also, included tests for the email smtp server.
</commit_message>
<xml_diff>
--- a/test_server/simulator_requirements.xlsx
+++ b/test_server/simulator_requirements.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="16395" windowHeight="10545" activeTab="1"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="16395" windowHeight="10545"/>
   </bookViews>
   <sheets>
     <sheet name="http" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
     <author>Centeno, Oscar</author>
   </authors>
   <commentList>
-    <comment ref="A14" authorId="0" shapeId="0">
+    <comment ref="A17" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="66">
   <si>
     <t>GET</t>
   </si>
@@ -256,6 +256,24 @@
     <t>{
   "id": "1"
 }</t>
+  </si>
+  <si>
+    <t>can match POST method, url and return status with response</t>
+  </si>
+  <si>
+    <t>can match PUT method, url and return status with response</t>
+  </si>
+  <si>
+    <t>can match DELETE method, url and return status with response</t>
+  </si>
+  <si>
+    <t>{ "message": "Hello World modified!" }</t>
+  </si>
+  <si>
+    <t>{ "message": "Hello World created!" }</t>
+  </si>
+  <si>
+    <t>{ "message": "Hello World deleted!" }</t>
   </si>
 </sst>
 </file>
@@ -394,8 +412,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H14" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Normal">
-  <autoFilter ref="A1:H14"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H17" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Normal">
+  <autoFilter ref="A1:H17"/>
   <tableColumns count="8">
     <tableColumn id="1" name="scenario" dataCellStyle="Normal"/>
     <tableColumn id="2" name="method" dataCellStyle="Normal"/>
@@ -724,10 +742,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -787,233 +805,293 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" t="s">
-        <v>0</v>
+        <v>60</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3">
-        <v>200</v>
+        <v>1</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5">
+        <v>201</v>
       </c>
       <c r="H3" t="s">
-        <v>12</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4" t="s">
-        <v>0</v>
+        <v>61</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4">
-        <v>403</v>
+        <v>1</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5">
+        <v>200</v>
       </c>
       <c r="H4" t="s">
-        <v>25</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F5" s="1"/>
-      <c r="G5" s="2">
-        <v>200</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>54</v>
+      <c r="A5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5">
+        <v>200</v>
+      </c>
+      <c r="H5" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
       </c>
-      <c r="E6" t="s">
-        <v>27</v>
-      </c>
       <c r="G6">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H6" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B7" t="s">
         <v>0</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>34</v>
+      </c>
+      <c r="F7" t="s">
+        <v>24</v>
       </c>
       <c r="G7">
-        <v>200</v>
+        <v>403</v>
       </c>
       <c r="H7" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" t="s">
-        <v>28</v>
-      </c>
-      <c r="G8">
-        <v>200</v>
-      </c>
-      <c r="H8" t="s">
-        <v>28</v>
+      <c r="A8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F8" s="1"/>
+      <c r="G8" s="2">
+        <v>200</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B9" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="E9" t="s">
+        <v>27</v>
       </c>
       <c r="G9">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="H9" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B10" t="s">
         <v>0</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="G10">
-        <v>404</v>
+        <v>200</v>
       </c>
       <c r="H10" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11" t="s">
-        <v>16</v>
+        <v>7</v>
+      </c>
+      <c r="E11" t="s">
+        <v>28</v>
       </c>
       <c r="G11">
         <v>200</v>
       </c>
       <c r="H11" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="B12" t="s">
         <v>0</v>
       </c>
       <c r="C12" t="s">
-        <v>41</v>
-      </c>
-      <c r="D12" t="s">
-        <v>55</v>
+        <v>6</v>
       </c>
       <c r="G12">
         <v>200</v>
       </c>
       <c r="H12" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="B13" t="s">
         <v>0</v>
       </c>
       <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13">
+        <v>404</v>
+      </c>
+      <c r="H13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" t="s">
+        <v>16</v>
+      </c>
+      <c r="G14">
+        <v>200</v>
+      </c>
+      <c r="H14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" t="s">
+        <v>55</v>
+      </c>
+      <c r="G15">
+        <v>200</v>
+      </c>
+      <c r="H15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" t="s">
         <v>33</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D16" t="s">
         <v>32</v>
       </c>
-      <c r="G13">
-        <v>200</v>
-      </c>
-      <c r="H13" t="s">
+      <c r="G16">
+        <v>200</v>
+      </c>
+      <c r="H16" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+    <row r="17" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B17" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C17" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="6" t="s">
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="G14" s="5">
-        <v>200</v>
-      </c>
-      <c r="H14" s="5" t="s">
+      <c r="G17" s="5">
+        <v>200</v>
+      </c>
+      <c r="H17" s="5" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1031,7 +1109,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>

</xml_diff>